<commit_message>
save file from csv to xlsx
</commit_message>
<xml_diff>
--- a/vulsList.xlsx
+++ b/vulsList.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11865"/>
+    <workbookView xWindow="0" yWindow="15" windowWidth="19200" windowHeight="11865" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="vulsHistory" sheetId="1" r:id="rId1"/>
     <sheet name="whiteList" sheetId="2" r:id="rId2"/>
-    <sheet name="blaskList" sheetId="3" r:id="rId3"/>
+    <sheet name="blackList" sheetId="3" r:id="rId3"/>
     <sheet name="run" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="141">
   <si>
     <t>wordpress</t>
   </si>
@@ -132,6 +132,342 @@
   <si>
     <t>risk</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/remote/?order_by=date&amp;order=desc</t>
+  </si>
+  <si>
+    <t>Th3 MMA mma.php Backdoor Arbitrary File Upload</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>Safari User-Assisted Applescript Exec Attack</t>
+  </si>
+  <si>
+    <t>osx</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/webapps/?order_by=date&amp;order=desc</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/local/?order_by=date&amp;order=desc</t>
+  </si>
+  <si>
+    <t>Mac OS X 10.9.5 / 10.10.5 - rsh/libmalloc Privilege Escalation</t>
+  </si>
+  <si>
+    <t>Windows 10 - pcap Driver Local Privilege Escalation</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/dos/?order_by=date&amp;order=desc</t>
+  </si>
+  <si>
+    <t>Win10Pcap - Local Privilege Escalation Vulnerability</t>
+  </si>
+  <si>
+    <t>https://www.hkcert.org/security-bulletin?p_p_id=3tech_list_security_bulletin_full_WAR_3tech_list_security_bulletin_fullportlet&amp;_3tech_list_security_bulletin_full_WAR_3tech_list_security_bulletin_fullportlet_cur=</t>
+  </si>
+  <si>
+    <t>Adobe Shockwave Player Remote Code Execution Vulnerabilitynew</t>
+  </si>
+  <si>
+    <t>PHP Phar Extension Multiple Vulnerabilitiesnew</t>
+  </si>
+  <si>
+    <t>Joomla Multiple SQL injection vulnerabilitiesnew</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/index.php?act=sec_bug</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems SQL注入漏洞(CVE-2015-6486)</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems跨站腳本漏洞(CVE-2015-6488)</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems任意文件上傳漏洞(CVE-2015-6491）</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems緩衝區溢出漏洞(CVE-2015-6492）</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems棧緩衝區溢出漏洞(CVE-2015-6490）</t>
+  </si>
+  <si>
+    <t>Adobe Shockwave Player內存破壞漏洞( CVE-2015-7649）</t>
+  </si>
+  <si>
+    <t>Apache HttpComponents HttpClient拒絕服務漏洞(CVE-2015-5262）</t>
+  </si>
+  <si>
+    <t>Cisco ASR 5000 PMIPv6拒絕服務漏洞(CVE-2015-6340）</t>
+  </si>
+  <si>
+    <t>SAP HANA hdbindexserver內存破壞漏洞(CVE-2015-7986）</t>
+  </si>
+  <si>
+    <t>OpenStack Neutron安全限制繞過漏洞(CVE-2015-5240）</t>
+  </si>
+  <si>
+    <t>ownCloud Desktop Client中間人攻擊漏洞(CVE-2015-4456)</t>
+  </si>
+  <si>
+    <t>PostgreSQL crypt函數拒絕服務漏洞(CVE-2015-5288）</t>
+  </si>
+  <si>
+    <t>Apple Xcode Swift安全漏洞(CVE-2015-7030)</t>
+  </si>
+  <si>
+    <t>PostgreSQL 棧緩衝區溢出漏洞(CVE-2015-5289）</t>
+  </si>
+  <si>
+    <t>ownCloud Server任意代碼執行漏洞(CVE-2015-7699)</t>
+  </si>
+  <si>
+    <t>ownCloud Desktop Client中間人攻擊漏洞(CVE-2015-7298)</t>
+  </si>
+  <si>
+    <t>ownCloud Server 目錄遍歷漏洞(CVE-2015-6670)</t>
+  </si>
+  <si>
+    <t>ownCloud Server 目錄遍歷漏洞(CVE-2015-6500)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-5942)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6976)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6977)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6978)</t>
+  </si>
+  <si>
+    <t>Apple iOS 雙重釋放漏洞(CVE-2015-6983)</t>
+  </si>
+  <si>
+    <t>Apple OS X libarchive符號鏈接攻擊漏洞(CVE-2015-6984)</t>
+  </si>
+  <si>
+    <t>Apple OS X ATS內存破壞漏洞(CVE-2015-6985)</t>
+  </si>
+  <si>
+    <t>Apple OS X File Bookmark拒絕服務漏洞(CVE-2015-6987)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X 任意代碼執行漏洞(CVE-2015-6988)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 內存破壞漏洞(CVE-2015-6989)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6990)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6991)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-6993)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X Dish Images內存破壞漏洞(CVE-2015-6994)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X Dish Images內存破壞漏洞(CVE-2015-6995)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 內存破壞漏洞(CVE-2015-6996)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 目錄遍歷漏洞(CVE-2015-7006)</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞(CVE-2015-7003)</t>
+  </si>
+  <si>
+    <t>Apple iOS BOM目錄遍歷漏洞(CVE-2015-7006)</t>
+  </si>
+  <si>
+    <t>Apple OS X Script Editor安全限制繞過漏洞(CVE-2015-7007)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-7008)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-7009)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-7010)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes 內存破壞漏洞(CVE-2015-7011)</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞(CVE-2015-7012)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes 內存破壞漏洞(CVE-2015-7013)</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞(CVE-2015-7014)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS&amp;nbsp;&amp;nbsp;堆緩衝區溢出漏洞(CVE-2015-7015)</t>
+  </si>
+  <si>
+    <t>Apple OS X 權限提升漏洞(CVE-2015-7016)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞(CVE-2015-7018)</t>
+  </si>
+  <si>
+    <t>Apple OS X Graphics Drivers信息泄露及拒絕服務漏洞(CVE-2015-7019)</t>
+  </si>
+  <si>
+    <t>Apple OS X Graphics Drivers信息泄露及拒絕服務漏洞(CVE-2015-7020)</t>
+  </si>
+  <si>
+    <t>Apple OS X Graphics Drivers內存破壞漏洞(CVE-2015-7023)</t>
+  </si>
+  <si>
+    <t>Apple iOS CFNetwork cookie改寫漏洞(CVE-2015-7023)</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞(CVE-2015-6992)</t>
+  </si>
+  <si>
+    <t>Apple iOS 任意代碼執行漏洞(CVE-2015-6986)</t>
+  </si>
+  <si>
+    <t>Apple iOS內存破壞漏洞(CVE-2015-6982)</t>
+  </si>
+  <si>
+    <t>Apple iOS內存破壞漏洞(CVE-2015-6981)</t>
+  </si>
+  <si>
+    <t>Apple iOS GasGauge 內存破壞漏洞(CVE-2015-6979)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/iTunes 內存破壞漏洞(CVE-2015-6975)</t>
+  </si>
+  <si>
+    <t>Apple OS X SecurityAgent安全限制繞過漏洞(CVE-2015-5943)</t>
+  </si>
+  <si>
+    <t>Apple OS X CoreText 內存破壞漏洞(CVE-2015-5944)</t>
+  </si>
+  <si>
+    <t>Apple OS X Sandbox權限提升漏洞(CVE-2015-5945)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 內存破壞漏洞(CVE-2015-6974)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X 任意代碼執行漏洞(CVE-2015-5940)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 內存破壞漏洞(CVE-2015-5939)</t>
+  </si>
+  <si>
+    <t>Apple OS X ImageIO 內存破壞漏洞(CVE-2015-5938)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS ImageIO 內存破壞漏洞(CVE-2015-5937)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS ImageIO 內存破壞漏洞(CVE-2015-5936)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS ImageIO 內存破壞漏洞(CVE-2015-5935)</t>
+  </si>
+  <si>
+    <t>Apple OS X Audio 內存破壞漏洞(CVE-2015-5934)</t>
+  </si>
+  <si>
+    <t>Apple OS X 內核權限提升漏洞(CVE-2015-5932)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes WebKit內存破壞漏洞(CVE-2015-5931)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes WebKit內存破壞漏洞(CVE-2015-5930)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes WebKit內存破壞漏洞(CVE-2015-5929)</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes WebKit內存破壞漏洞(CVE-2015-5928)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS FontParser 內存破壞漏洞(CVE-2015-5927)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS CoreGraphics組件內存破壞漏洞(CVE-2015-5926)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS CoreGraphics組件內存破壞漏洞(CVE-2015-5925)</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X OpenGL內存破壞漏洞(CVE-2015-5924)</t>
+  </si>
+  <si>
+    <t>Apple Mac EFI未授權訪問漏洞(CVE-2015-7035)</t>
+  </si>
+  <si>
+    <t>Apple OS X Server訪問限制繞過漏洞(CVE-2015-7031)</t>
+  </si>
+  <si>
+    <t>Apple iOS Telephony信息泄露漏洞(CVE-2015-7022)</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞(CVE-2015-7017)</t>
+  </si>
+  <si>
+    <t>Apple iOS內存破壞漏洞(CVE-2015-7005)</t>
+  </si>
+  <si>
+    <t>Apple iOS內核拒絕服務漏洞(CVE-2015-7004)</t>
+  </si>
+  <si>
+    <t>Apple iOS 信息泄露漏洞(CVE-2015-7000)</t>
+  </si>
+  <si>
+    <t>Apple iOS OCSP證書驗證漏洞(CVE-2015-6999)</t>
+  </si>
+  <si>
+    <t>Apple iOS X.509證書驗證漏洞(CVE-2015-6997)</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance拒絕服務漏洞(CVE-2015-6324)</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance拒絕服務漏洞(CVE-2015-6325)</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance拒絕服務漏洞(CVE-2015-6326)</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance拒絕服務漏洞(CVE-2015-6327)</t>
+  </si>
+  <si>
+    <t>Cisco FireSIGHT Management Center任意命令執行漏洞(CVE-2015-6335)</t>
   </si>
 </sst>
 </file>
@@ -184,7 +520,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -193,6 +529,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,7 +829,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -689,14 +1028,1352 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C266"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="37.625" customWidth="1"/>
+    <col min="2" max="2" width="82.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B16" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B20" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B22" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B25" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B28" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B29" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B30" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B31" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B32" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B33" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B34" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B35" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B36" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B38" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B39" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B40" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B42" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B43" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B46" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B48" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B49" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B50" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B51" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B52" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B53" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B54" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B56" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B57" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B58" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B61" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B62" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B63" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B64" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B65" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B66" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B67" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B68" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B69" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B70" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B71" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B72" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B73" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B74" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B75" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B76" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B77" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B78" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B79" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B80" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B81" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B82" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B83" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B84" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B85" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B86" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B87" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B88" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B89" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B90" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B91" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B92" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B93" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B94" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B95" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B96" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B97" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B98" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B99" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B100" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B101" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B102" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B103" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B104" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B105" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B106" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B107" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" s="3"/>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" s="3"/>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" s="3"/>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" s="3"/>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" s="3"/>
+    </row>
+    <row r="113" spans="1:1">
+      <c r="A113" s="3"/>
+    </row>
+    <row r="114" spans="1:1">
+      <c r="A114" s="3"/>
+    </row>
+    <row r="115" spans="1:1">
+      <c r="A115" s="3"/>
+    </row>
+    <row r="116" spans="1:1">
+      <c r="A116" s="3"/>
+    </row>
+    <row r="117" spans="1:1">
+      <c r="A117" s="3"/>
+    </row>
+    <row r="118" spans="1:1">
+      <c r="A118" s="3"/>
+    </row>
+    <row r="119" spans="1:1">
+      <c r="A119" s="3"/>
+    </row>
+    <row r="120" spans="1:1">
+      <c r="A120" s="3"/>
+    </row>
+    <row r="121" spans="1:1">
+      <c r="A121" s="3"/>
+    </row>
+    <row r="122" spans="1:1">
+      <c r="A122" s="3"/>
+    </row>
+    <row r="123" spans="1:1">
+      <c r="A123" s="3"/>
+    </row>
+    <row r="124" spans="1:1">
+      <c r="A124" s="3"/>
+    </row>
+    <row r="125" spans="1:1">
+      <c r="A125" s="3"/>
+    </row>
+    <row r="126" spans="1:1">
+      <c r="A126" s="3"/>
+    </row>
+    <row r="127" spans="1:1">
+      <c r="A127" s="3"/>
+    </row>
+    <row r="128" spans="1:1">
+      <c r="A128" s="3"/>
+    </row>
+    <row r="129" spans="1:1">
+      <c r="A129" s="3"/>
+    </row>
+    <row r="130" spans="1:1">
+      <c r="A130" s="3"/>
+    </row>
+    <row r="131" spans="1:1">
+      <c r="A131" s="3"/>
+    </row>
+    <row r="132" spans="1:1">
+      <c r="A132" s="3"/>
+    </row>
+    <row r="133" spans="1:1">
+      <c r="A133" s="3"/>
+    </row>
+    <row r="134" spans="1:1">
+      <c r="A134" s="3"/>
+    </row>
+    <row r="135" spans="1:1">
+      <c r="A135" s="3"/>
+    </row>
+    <row r="136" spans="1:1">
+      <c r="A136" s="3"/>
+    </row>
+    <row r="137" spans="1:1">
+      <c r="A137" s="3"/>
+    </row>
+    <row r="138" spans="1:1">
+      <c r="A138" s="3"/>
+    </row>
+    <row r="139" spans="1:1">
+      <c r="A139" s="3"/>
+    </row>
+    <row r="140" spans="1:1">
+      <c r="A140" s="3"/>
+    </row>
+    <row r="141" spans="1:1">
+      <c r="A141" s="3"/>
+    </row>
+    <row r="142" spans="1:1">
+      <c r="A142" s="3"/>
+    </row>
+    <row r="143" spans="1:1">
+      <c r="A143" s="3"/>
+    </row>
+    <row r="144" spans="1:1">
+      <c r="A144" s="3"/>
+    </row>
+    <row r="145" spans="1:1">
+      <c r="A145" s="3"/>
+    </row>
+    <row r="146" spans="1:1">
+      <c r="A146" s="3"/>
+    </row>
+    <row r="147" spans="1:1">
+      <c r="A147" s="3"/>
+    </row>
+    <row r="148" spans="1:1">
+      <c r="A148" s="3"/>
+    </row>
+    <row r="149" spans="1:1">
+      <c r="A149" s="3"/>
+    </row>
+    <row r="150" spans="1:1">
+      <c r="A150" s="3"/>
+    </row>
+    <row r="151" spans="1:1">
+      <c r="A151" s="3"/>
+    </row>
+    <row r="152" spans="1:1">
+      <c r="A152" s="3"/>
+    </row>
+    <row r="153" spans="1:1">
+      <c r="A153" s="3"/>
+    </row>
+    <row r="154" spans="1:1">
+      <c r="A154" s="3"/>
+    </row>
+    <row r="155" spans="1:1">
+      <c r="A155" s="3"/>
+    </row>
+    <row r="156" spans="1:1">
+      <c r="A156" s="3"/>
+    </row>
+    <row r="157" spans="1:1">
+      <c r="A157" s="3"/>
+    </row>
+    <row r="158" spans="1:1">
+      <c r="A158" s="3"/>
+    </row>
+    <row r="159" spans="1:1">
+      <c r="A159" s="3"/>
+    </row>
+    <row r="160" spans="1:1">
+      <c r="A160" s="3"/>
+    </row>
+    <row r="161" spans="1:1">
+      <c r="A161" s="3"/>
+    </row>
+    <row r="162" spans="1:1">
+      <c r="A162" s="3"/>
+    </row>
+    <row r="163" spans="1:1">
+      <c r="A163" s="3"/>
+    </row>
+    <row r="164" spans="1:1">
+      <c r="A164" s="3"/>
+    </row>
+    <row r="165" spans="1:1">
+      <c r="A165" s="3"/>
+    </row>
+    <row r="166" spans="1:1">
+      <c r="A166" s="3"/>
+    </row>
+    <row r="167" spans="1:1">
+      <c r="A167" s="3"/>
+    </row>
+    <row r="168" spans="1:1">
+      <c r="A168" s="3"/>
+    </row>
+    <row r="169" spans="1:1">
+      <c r="A169" s="3"/>
+    </row>
+    <row r="170" spans="1:1">
+      <c r="A170" s="3"/>
+    </row>
+    <row r="171" spans="1:1">
+      <c r="A171" s="3"/>
+    </row>
+    <row r="172" spans="1:1">
+      <c r="A172" s="3"/>
+    </row>
+    <row r="173" spans="1:1">
+      <c r="A173" s="3"/>
+    </row>
+    <row r="174" spans="1:1">
+      <c r="A174" s="3"/>
+    </row>
+    <row r="175" spans="1:1">
+      <c r="A175" s="3"/>
+    </row>
+    <row r="176" spans="1:1">
+      <c r="A176" s="3"/>
+    </row>
+    <row r="177" spans="1:1">
+      <c r="A177" s="3"/>
+    </row>
+    <row r="178" spans="1:1">
+      <c r="A178" s="3"/>
+    </row>
+    <row r="179" spans="1:1">
+      <c r="A179" s="3"/>
+    </row>
+    <row r="180" spans="1:1">
+      <c r="A180" s="3"/>
+    </row>
+    <row r="181" spans="1:1">
+      <c r="A181" s="3"/>
+    </row>
+    <row r="182" spans="1:1">
+      <c r="A182" s="3"/>
+    </row>
+    <row r="183" spans="1:1">
+      <c r="A183" s="3"/>
+    </row>
+    <row r="184" spans="1:1">
+      <c r="A184" s="3"/>
+    </row>
+    <row r="185" spans="1:1">
+      <c r="A185" s="3"/>
+    </row>
+    <row r="186" spans="1:1">
+      <c r="A186" s="3"/>
+    </row>
+    <row r="187" spans="1:1">
+      <c r="A187" s="3"/>
+    </row>
+    <row r="188" spans="1:1">
+      <c r="A188" s="3"/>
+    </row>
+    <row r="189" spans="1:1">
+      <c r="A189" s="3"/>
+    </row>
+    <row r="190" spans="1:1">
+      <c r="A190" s="3"/>
+    </row>
+    <row r="191" spans="1:1">
+      <c r="A191" s="3"/>
+    </row>
+    <row r="192" spans="1:1">
+      <c r="A192" s="3"/>
+    </row>
+    <row r="193" spans="1:1">
+      <c r="A193" s="3"/>
+    </row>
+    <row r="194" spans="1:1">
+      <c r="A194" s="3"/>
+    </row>
+    <row r="195" spans="1:1">
+      <c r="A195" s="3"/>
+    </row>
+    <row r="196" spans="1:1">
+      <c r="A196" s="3"/>
+    </row>
+    <row r="197" spans="1:1">
+      <c r="A197" s="3"/>
+    </row>
+    <row r="198" spans="1:1">
+      <c r="A198" s="3"/>
+    </row>
+    <row r="199" spans="1:1">
+      <c r="A199" s="3"/>
+    </row>
+    <row r="200" spans="1:1">
+      <c r="A200" s="3"/>
+    </row>
+    <row r="201" spans="1:1">
+      <c r="A201" s="3"/>
+    </row>
+    <row r="202" spans="1:1">
+      <c r="A202" s="3"/>
+    </row>
+    <row r="203" spans="1:1">
+      <c r="A203" s="3"/>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" s="3"/>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" s="3"/>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" s="3"/>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" s="3"/>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" s="3"/>
+    </row>
+    <row r="209" spans="1:1">
+      <c r="A209" s="3"/>
+    </row>
+    <row r="210" spans="1:1">
+      <c r="A210" s="3"/>
+    </row>
+    <row r="211" spans="1:1">
+      <c r="A211" s="3"/>
+    </row>
+    <row r="212" spans="1:1">
+      <c r="A212" s="3"/>
+    </row>
+    <row r="213" spans="1:1">
+      <c r="A213" s="3"/>
+    </row>
+    <row r="214" spans="1:1">
+      <c r="A214" s="3"/>
+    </row>
+    <row r="215" spans="1:1">
+      <c r="A215" s="3"/>
+    </row>
+    <row r="216" spans="1:1">
+      <c r="A216" s="3"/>
+    </row>
+    <row r="217" spans="1:1">
+      <c r="A217" s="3"/>
+    </row>
+    <row r="218" spans="1:1">
+      <c r="A218" s="3"/>
+    </row>
+    <row r="219" spans="1:1">
+      <c r="A219" s="3"/>
+    </row>
+    <row r="220" spans="1:1">
+      <c r="A220" s="3"/>
+    </row>
+    <row r="221" spans="1:1">
+      <c r="A221" s="3"/>
+    </row>
+    <row r="222" spans="1:1">
+      <c r="A222" s="3"/>
+    </row>
+    <row r="223" spans="1:1">
+      <c r="A223" s="3"/>
+    </row>
+    <row r="224" spans="1:1">
+      <c r="A224" s="3"/>
+    </row>
+    <row r="225" spans="1:1">
+      <c r="A225" s="3"/>
+    </row>
+    <row r="226" spans="1:1">
+      <c r="A226" s="3"/>
+    </row>
+    <row r="227" spans="1:1">
+      <c r="A227" s="3"/>
+    </row>
+    <row r="228" spans="1:1">
+      <c r="A228" s="3"/>
+    </row>
+    <row r="229" spans="1:1">
+      <c r="A229" s="3"/>
+    </row>
+    <row r="230" spans="1:1">
+      <c r="A230" s="3"/>
+    </row>
+    <row r="231" spans="1:1">
+      <c r="A231" s="3"/>
+    </row>
+    <row r="232" spans="1:1">
+      <c r="A232" s="3"/>
+    </row>
+    <row r="233" spans="1:1">
+      <c r="A233" s="3"/>
+    </row>
+    <row r="234" spans="1:1">
+      <c r="A234" s="3"/>
+    </row>
+    <row r="235" spans="1:1">
+      <c r="A235" s="3"/>
+    </row>
+    <row r="236" spans="1:1">
+      <c r="A236" s="3"/>
+    </row>
+    <row r="237" spans="1:1">
+      <c r="A237" s="3"/>
+    </row>
+    <row r="238" spans="1:1">
+      <c r="A238" s="3"/>
+    </row>
+    <row r="239" spans="1:1">
+      <c r="A239" s="3"/>
+    </row>
+    <row r="240" spans="1:1">
+      <c r="A240" s="3"/>
+    </row>
+    <row r="241" spans="1:1">
+      <c r="A241" s="3"/>
+    </row>
+    <row r="242" spans="1:1">
+      <c r="A242" s="3"/>
+    </row>
+    <row r="243" spans="1:1">
+      <c r="A243" s="3"/>
+    </row>
+    <row r="244" spans="1:1">
+      <c r="A244" s="3"/>
+    </row>
+    <row r="245" spans="1:1">
+      <c r="A245" s="3"/>
+    </row>
+    <row r="246" spans="1:1">
+      <c r="A246" s="3"/>
+    </row>
+    <row r="247" spans="1:1">
+      <c r="A247" s="3"/>
+    </row>
+    <row r="248" spans="1:1">
+      <c r="A248" s="3"/>
+    </row>
+    <row r="249" spans="1:1">
+      <c r="A249" s="3"/>
+    </row>
+    <row r="250" spans="1:1">
+      <c r="A250" s="3"/>
+    </row>
+    <row r="251" spans="1:1">
+      <c r="A251" s="3"/>
+    </row>
+    <row r="252" spans="1:1">
+      <c r="A252" s="3"/>
+    </row>
+    <row r="253" spans="1:1">
+      <c r="A253" s="3"/>
+    </row>
+    <row r="254" spans="1:1">
+      <c r="A254" s="3"/>
+    </row>
+    <row r="255" spans="1:1">
+      <c r="A255" s="3"/>
+    </row>
+    <row r="256" spans="1:1">
+      <c r="A256" s="3"/>
+    </row>
+    <row r="257" spans="1:1">
+      <c r="A257" s="3"/>
+    </row>
+    <row r="258" spans="1:1">
+      <c r="A258" s="3"/>
+    </row>
+    <row r="259" spans="1:1">
+      <c r="A259" s="3"/>
+    </row>
+    <row r="260" spans="1:1">
+      <c r="A260" s="3"/>
+    </row>
+    <row r="261" spans="1:1">
+      <c r="A261" s="3"/>
+    </row>
+    <row r="262" spans="1:1">
+      <c r="A262" s="3"/>
+    </row>
+    <row r="263" spans="1:1">
+      <c r="A263" s="3"/>
+    </row>
+    <row r="264" spans="1:1">
+      <c r="A264" s="3"/>
+    </row>
+    <row r="265" spans="1:1">
+      <c r="A265" s="3"/>
+    </row>
+    <row r="266" spans="1:1">
+      <c r="A266" s="3"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add exploitDB and hkcert CVE
</commit_message>
<xml_diff>
--- a/vulsList.xlsx
+++ b/vulsList.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="298">
   <si>
     <t>wordpress</t>
   </si>
@@ -134,180 +134,811 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Platform</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>CVE</t>
+  </si>
+  <si>
+    <t>Th3 MMA mma.php Backdoor Arbitrary File Upload</t>
+  </si>
+  <si>
+    <t>php</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/exploits/38541/</t>
+  </si>
+  <si>
+    <t>CVE-N/A</t>
+  </si>
+  <si>
+    <t>Safari User-Assisted Applescript Exec Attack</t>
+  </si>
+  <si>
+    <t>osx</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/exploits/38535/</t>
+  </si>
+  <si>
+    <t>CVE-2015-7007</t>
+  </si>
+  <si>
+    <t>Mac OS X 10.9.5 / 10.10.5 - rsh/libmalloc Privilege Escalation</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/exploits/38540/</t>
+  </si>
+  <si>
+    <t>CVE-2015-5889</t>
+  </si>
+  <si>
+    <t>Windows 10 - pcap Driver Local Privilege Escalation</t>
+  </si>
+  <si>
+    <t>windows</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/exploits/38533/</t>
+  </si>
+  <si>
+    <t>Win10Pcap - Local Privilege Escalation Vulnerability</t>
+  </si>
+  <si>
+    <t>https://www.exploit-db.com/exploits/38542/</t>
+  </si>
+  <si>
+    <t>Adobe Shockwave Player Remote Code Execution Vulnerabilitynew</t>
+  </si>
+  <si>
+    <t>https://www.hkcert.org/my_url/en/alert/15102802</t>
+  </si>
+  <si>
+    <t>CVE-2015-7649,</t>
+  </si>
+  <si>
+    <t>PHP Phar Extension Multiple Vulnerabilitiesnew</t>
+  </si>
+  <si>
+    <t>https://www.hkcert.org/my_url/en/alert/15102801</t>
+  </si>
+  <si>
+    <t>CVE-2015-7803,CVE-2015-7804,</t>
+  </si>
+  <si>
+    <t>Joomla Multiple SQL injection vulnerabilitiesnew</t>
+  </si>
+  <si>
+    <t>https://www.hkcert.org/my_url/en/alert/15102701</t>
+  </si>
+  <si>
+    <t>CVE-2015-7297,CVE-2015-7857,CVE-2015-7858,</t>
+  </si>
+  <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems SQL注入漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31392</t>
+  </si>
+  <si>
     <t>CVE-2015-6486</t>
   </si>
   <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems跨站腳本漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31391</t>
+  </si>
+  <si>
     <t>CVE-2015-6488</t>
   </si>
   <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems任意文件上傳漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31390</t>
+  </si>
+  <si>
     <t>CVE-2015-6491</t>
   </si>
   <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems緩衝區溢出漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31389</t>
+  </si>
+  <si>
     <t>CVE-2015-6492</t>
   </si>
   <si>
+    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems棧緩衝區溢出漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31388</t>
+  </si>
+  <si>
     <t>CVE-2015-6490</t>
   </si>
   <si>
+    <t>Adobe Shockwave Player內存破壞漏洞(</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31387</t>
+  </si>
+  <si>
     <t>CVE-2015-7649</t>
   </si>
   <si>
+    <t>Apache HttpComponents HttpClient拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31386</t>
+  </si>
+  <si>
     <t>CVE-2015-5262</t>
   </si>
   <si>
+    <t>Cisco ASR 5000 PMIPv6拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31385</t>
+  </si>
+  <si>
     <t>CVE-2015-6340</t>
   </si>
   <si>
+    <t>SAP HANA hdbindexserver內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31384</t>
+  </si>
+  <si>
     <t>CVE-2015-7986</t>
   </si>
   <si>
+    <t>OpenStack Neutron安全限制繞過漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31383</t>
+  </si>
+  <si>
     <t>CVE-2015-5240</t>
   </si>
   <si>
+    <t>ownCloud Desktop Client中間人攻擊漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31312</t>
+  </si>
+  <si>
     <t>CVE-2015-4456</t>
   </si>
   <si>
+    <t>PostgreSQL crypt函數拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31311</t>
+  </si>
+  <si>
     <t>CVE-2015-5288</t>
   </si>
   <si>
+    <t>Apple Xcode Swift安全漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31310</t>
+  </si>
+  <si>
     <t>CVE-2015-7030</t>
   </si>
   <si>
+    <t>PostgreSQL 棧緩衝區溢出漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31309</t>
+  </si>
+  <si>
     <t>CVE-2015-5289</t>
   </si>
   <si>
+    <t>ownCloud Server任意代碼執行漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31308</t>
+  </si>
+  <si>
     <t>CVE-2015-7699</t>
   </si>
   <si>
+    <t>http://www.nsfocus.net/vulndb/31307</t>
+  </si>
+  <si>
     <t>CVE-2015-7298</t>
   </si>
   <si>
+    <t>ownCloud Server 目錄遍歷漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31306</t>
+  </si>
+  <si>
     <t>CVE-2015-6670</t>
   </si>
   <si>
+    <t>http://www.nsfocus.net/vulndb/31305</t>
+  </si>
+  <si>
     <t>CVE-2015-6500</t>
   </si>
   <si>
-    <t>Date</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Title</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Platform</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Source</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>CVE</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems SQL注入漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31392</t>
-  </si>
-  <si>
-    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems跨站腳本漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31391</t>
-  </si>
-  <si>
-    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems任意文件上傳漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31390</t>
-  </si>
-  <si>
-    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems緩衝區溢出漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31389</t>
-  </si>
-  <si>
-    <t>Rockwell Automation Micrologix 1100/1400 PLC Systems棧緩衝區溢出漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31388</t>
-  </si>
-  <si>
-    <t>Adobe Shockwave Player內存破壞漏洞(</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31387</t>
-  </si>
-  <si>
-    <t>Apache HttpComponents HttpClient拒絕服務漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31386</t>
-  </si>
-  <si>
-    <t>Cisco ASR 5000 PMIPv6拒絕服務漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31385</t>
-  </si>
-  <si>
-    <t>SAP HANA hdbindexserver內存破壞漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31384</t>
-  </si>
-  <si>
-    <t>OpenStack Neutron安全限制繞過漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31383</t>
-  </si>
-  <si>
-    <t>ownCloud Desktop Client中間人攻擊漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31312</t>
-  </si>
-  <si>
-    <t>PostgreSQL crypt函數拒絕服務漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31311</t>
-  </si>
-  <si>
-    <t>Apple Xcode Swift安全漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31310</t>
-  </si>
-  <si>
-    <t>PostgreSQL 棧緩衝區溢出漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31309</t>
-  </si>
-  <si>
-    <t>ownCloud Server任意代碼執行漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31308</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31307</t>
-  </si>
-  <si>
-    <t>ownCloud Server 目錄遍歷漏洞</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31306</t>
-  </si>
-  <si>
-    <t>http://www.nsfocus.net/vulndb/31305</t>
+    <t>Apple iOS/OS X FontParser 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31382</t>
+  </si>
+  <si>
+    <t>CVE-2015-5942</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31381</t>
+  </si>
+  <si>
+    <t>CVE-2015-6976</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31380</t>
+  </si>
+  <si>
+    <t>CVE-2015-6977</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31379</t>
+  </si>
+  <si>
+    <t>CVE-2015-6978</t>
+  </si>
+  <si>
+    <t>Apple iOS 雙重釋放漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31378</t>
+  </si>
+  <si>
+    <t>CVE-2015-6983</t>
+  </si>
+  <si>
+    <t>Apple OS X libarchive符號鏈接攻擊漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31377</t>
+  </si>
+  <si>
+    <t>CVE-2015-6984</t>
+  </si>
+  <si>
+    <t>Apple OS X ATS內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31376</t>
+  </si>
+  <si>
+    <t>CVE-2015-6985</t>
+  </si>
+  <si>
+    <t>Apple OS X File Bookmark拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31375</t>
+  </si>
+  <si>
+    <t>CVE-2015-6987</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X 任意代碼執行漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31374</t>
+  </si>
+  <si>
+    <t>CVE-2015-6988</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31373</t>
+  </si>
+  <si>
+    <t>CVE-2015-6989</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31372</t>
+  </si>
+  <si>
+    <t>CVE-2015-6990</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31371</t>
+  </si>
+  <si>
+    <t>CVE-2015-6991</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31370</t>
+  </si>
+  <si>
+    <t>CVE-2015-6993</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X Dish Images內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31369</t>
+  </si>
+  <si>
+    <t>CVE-2015-6994</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31368</t>
+  </si>
+  <si>
+    <t>CVE-2015-6995</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31367</t>
+  </si>
+  <si>
+    <t>CVE-2015-6996</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS 目錄遍歷漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31366</t>
+  </si>
+  <si>
+    <t>CVE-2015-7006</t>
+  </si>
+  <si>
+    <t>Apple iOS/Safari/iTunes 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31365</t>
+  </si>
+  <si>
+    <t>CVE-2015-7003</t>
+  </si>
+  <si>
+    <t>Apple iOS BOM目錄遍歷漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31364</t>
+  </si>
+  <si>
+    <t>Apple OS X Script Editor安全限制繞過漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31363</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31362</t>
+  </si>
+  <si>
+    <t>CVE-2015-7008</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31361</t>
+  </si>
+  <si>
+    <t>CVE-2015-7009</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31360</t>
+  </si>
+  <si>
+    <t>CVE-2015-7010</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31359</t>
+  </si>
+  <si>
+    <t>CVE-2015-7011</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31358</t>
+  </si>
+  <si>
+    <t>CVE-2015-7012</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31357</t>
+  </si>
+  <si>
+    <t>CVE-2015-7013</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31356</t>
+  </si>
+  <si>
+    <t>CVE-2015-7014</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS&amp;nbsp;&amp;nbsp;堆緩衝區溢出漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31355</t>
+  </si>
+  <si>
+    <t>CVE-2015-7015</t>
+  </si>
+  <si>
+    <t>Apple OS X 權限提升漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31354</t>
+  </si>
+  <si>
+    <t>CVE-2015-7016</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31353</t>
+  </si>
+  <si>
+    <t>CVE-2015-7018</t>
+  </si>
+  <si>
+    <t>Apple OS X Graphics Drivers信息泄露及拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31352</t>
+  </si>
+  <si>
+    <t>CVE-2015-7019</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31351</t>
+  </si>
+  <si>
+    <t>CVE-2015-7020</t>
+  </si>
+  <si>
+    <t>Apple OS X Graphics Drivers內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31350</t>
+  </si>
+  <si>
+    <t>CVE-2015-7023</t>
+  </si>
+  <si>
+    <t>Apple iOS CFNetwork cookie改寫漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31349</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31348</t>
+  </si>
+  <si>
+    <t>CVE-2015-6992</t>
+  </si>
+  <si>
+    <t>Apple iOS 任意代碼執行漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31347</t>
+  </si>
+  <si>
+    <t>CVE-2015-6986</t>
+  </si>
+  <si>
+    <t>Apple iOS內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31346</t>
+  </si>
+  <si>
+    <t>CVE-2015-6982</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31345</t>
+  </si>
+  <si>
+    <t>CVE-2015-6981</t>
+  </si>
+  <si>
+    <t>Apple iOS GasGauge 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31344</t>
+  </si>
+  <si>
+    <t>CVE-2015-6979</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/iTunes 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31343</t>
+  </si>
+  <si>
+    <t>CVE-2015-6975</t>
+  </si>
+  <si>
+    <t>Apple OS X SecurityAgent安全限制繞過漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31342</t>
+  </si>
+  <si>
+    <t>CVE-2015-5943</t>
+  </si>
+  <si>
+    <t>Apple OS X CoreText 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31341</t>
+  </si>
+  <si>
+    <t>CVE-2015-5944</t>
+  </si>
+  <si>
+    <t>Apple OS X Sandbox權限提升漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31340</t>
+  </si>
+  <si>
+    <t>CVE-2015-5945</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31339</t>
+  </si>
+  <si>
+    <t>CVE-2015-6974</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31338</t>
+  </si>
+  <si>
+    <t>CVE-2015-5940</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31337</t>
+  </si>
+  <si>
+    <t>CVE-2015-5939</t>
+  </si>
+  <si>
+    <t>Apple OS X ImageIO 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31336</t>
+  </si>
+  <si>
+    <t>CVE-2015-5938</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS ImageIO 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31335</t>
+  </si>
+  <si>
+    <t>CVE-2015-5937</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31334</t>
+  </si>
+  <si>
+    <t>CVE-2015-5936</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31333</t>
+  </si>
+  <si>
+    <t>CVE-2015-5935</t>
+  </si>
+  <si>
+    <t>Apple OS X Audio 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31332</t>
+  </si>
+  <si>
+    <t>CVE-2015-5934</t>
+  </si>
+  <si>
+    <t>Apple OS X 內核權限提升漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31330</t>
+  </si>
+  <si>
+    <t>CVE-2015-5932</t>
+  </si>
+  <si>
+    <t>Apple Safari/iTunes WebKit內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31329</t>
+  </si>
+  <si>
+    <t>CVE-2015-5931</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31328</t>
+  </si>
+  <si>
+    <t>CVE-2015-5930</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31327</t>
+  </si>
+  <si>
+    <t>CVE-2015-5929</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31326</t>
+  </si>
+  <si>
+    <t>CVE-2015-5928</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS FontParser 內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31325</t>
+  </si>
+  <si>
+    <t>CVE-2015-5927</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X/watchOS CoreGraphics組件內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31324</t>
+  </si>
+  <si>
+    <t>CVE-2015-5926</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31323</t>
+  </si>
+  <si>
+    <t>CVE-2015-5925</t>
+  </si>
+  <si>
+    <t>Apple iOS/OS X OpenGL內存破壞漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31322</t>
+  </si>
+  <si>
+    <t>CVE-2015-5924</t>
+  </si>
+  <si>
+    <t>Apple Mac EFI未授權訪問漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31321</t>
+  </si>
+  <si>
+    <t>CVE-2015-7035</t>
+  </si>
+  <si>
+    <t>Apple OS X Server訪問限制繞過漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31320</t>
+  </si>
+  <si>
+    <t>CVE-2015-7031</t>
+  </si>
+  <si>
+    <t>Apple iOS Telephony信息泄露漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31319</t>
+  </si>
+  <si>
+    <t>CVE-2015-7022</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31318</t>
+  </si>
+  <si>
+    <t>CVE-2015-7017</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31317</t>
+  </si>
+  <si>
+    <t>CVE-2015-7005</t>
+  </si>
+  <si>
+    <t>Apple iOS內核拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31316</t>
+  </si>
+  <si>
+    <t>CVE-2015-7004</t>
+  </si>
+  <si>
+    <t>Apple iOS 信息泄露漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31315</t>
+  </si>
+  <si>
+    <t>CVE-2015-7000</t>
+  </si>
+  <si>
+    <t>Apple iOS OCSP證書驗證漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31314</t>
+  </si>
+  <si>
+    <t>CVE-2015-6999</t>
+  </si>
+  <si>
+    <t>Apple iOS X.509證書驗證漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31313</t>
+  </si>
+  <si>
+    <t>CVE-2015-6997</t>
+  </si>
+  <si>
+    <t>Cisco Adaptive Security Appliance拒絕服務漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31304</t>
+  </si>
+  <si>
+    <t>CVE-2015-6324</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31303</t>
+  </si>
+  <si>
+    <t>CVE-2015-6325</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31302</t>
+  </si>
+  <si>
+    <t>CVE-2015-6326</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31301</t>
+  </si>
+  <si>
+    <t>CVE-2015-6327</t>
+  </si>
+  <si>
+    <t>Cisco FireSIGHT Management Center任意命令執行漏洞</t>
+  </si>
+  <si>
+    <t>http://www.nsfocus.net/vulndb/31300</t>
+  </si>
+  <si>
+    <t>CVE-2015-6335</t>
   </si>
 </sst>
 </file>
@@ -874,99 +1505,114 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5"/>
+  <sheetFormatPr defaultColWidth="18.5" defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="18.75" customWidth="1"/>
-    <col min="2" max="2" width="78.75" customWidth="1"/>
-    <col min="3" max="3" width="22.75" customWidth="1"/>
-    <col min="4" max="4" width="40.5" customWidth="1"/>
+    <col min="1" max="1" width="13.5" customWidth="1"/>
+    <col min="2" max="2" width="53.125" customWidth="1"/>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="40.25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="B1" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="C1" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E1" t="s">
-        <v>51</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="3">
-        <v>42305</v>
+        <v>42304</v>
       </c>
       <c r="B2" t="s">
-        <v>52</v>
+        <v>34</v>
+      </c>
+      <c r="C2" t="s">
+        <v>35</v>
       </c>
       <c r="D2" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="E2" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="3">
-        <v>42305</v>
+        <v>42303</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>38</v>
+      </c>
+      <c r="C3" t="s">
+        <v>39</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>40</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="3">
-        <v>42305</v>
+        <v>42304</v>
       </c>
       <c r="B4" t="s">
-        <v>56</v>
+        <v>42</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
       </c>
       <c r="D4" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="3">
-        <v>42305</v>
+        <v>42303</v>
       </c>
       <c r="B5" t="s">
-        <v>58</v>
+        <v>45</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>59</v>
+        <v>47</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="3">
-        <v>42305</v>
+        <v>42304</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
       </c>
       <c r="D6" t="s">
-        <v>61</v>
+        <v>49</v>
       </c>
       <c r="E6" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -974,13 +1620,13 @@
         <v>42305</v>
       </c>
       <c r="B7" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
       <c r="E7" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -988,27 +1634,27 @@
         <v>42305</v>
       </c>
       <c r="B8" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s">
-        <v>35</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="3">
-        <v>42305</v>
+        <v>42304</v>
       </c>
       <c r="B9" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>36</v>
+        <v>58</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1016,13 +1662,13 @@
         <v>42305</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="E10" t="s">
-        <v>37</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1030,102 +1676,102 @@
         <v>42305</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="D11" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="E11" t="s">
-        <v>38</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B12" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B13" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="D13" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="E13" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B14" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="E14" t="s">
-        <v>41</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="D15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E15" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B16" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="D16" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="E16" t="s">
-        <v>43</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B17" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D17" t="s">
+        <v>81</v>
+      </c>
+      <c r="E17" t="s">
         <v>82</v>
-      </c>
-      <c r="E17" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="3">
-        <v>42304</v>
+        <v>42305</v>
       </c>
       <c r="B18" t="s">
         <v>83</v>
@@ -1134,300 +1780,1202 @@
         <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="3">
+        <v>42305</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="3">
         <v>42304</v>
       </c>
-      <c r="B19" t="s">
-        <v>83</v>
-      </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="3"/>
+      <c r="B20" t="s">
+        <v>89</v>
+      </c>
+      <c r="D20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E20" t="s">
+        <v>91</v>
+      </c>
     </row>
     <row r="21" spans="1:5">
-      <c r="A21" s="3"/>
+      <c r="A21" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B21" t="s">
+        <v>92</v>
+      </c>
+      <c r="D21" t="s">
+        <v>93</v>
+      </c>
+      <c r="E21" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B22" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="23" spans="1:5">
-      <c r="A23" s="3"/>
+      <c r="A23" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B23" t="s">
+        <v>98</v>
+      </c>
+      <c r="D23" t="s">
+        <v>99</v>
+      </c>
+      <c r="E23" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="24" spans="1:5">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B24" t="s">
+        <v>101</v>
+      </c>
+      <c r="D24" t="s">
+        <v>102</v>
+      </c>
+      <c r="E24" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="25" spans="1:5">
-      <c r="A25" s="3"/>
+      <c r="A25" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="26" spans="1:5">
-      <c r="A26" s="3"/>
+      <c r="A26" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D26" t="s">
+        <v>107</v>
+      </c>
+      <c r="E26" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="27" spans="1:5">
-      <c r="A27" s="3"/>
+      <c r="A27" s="3">
+        <v>42304</v>
+      </c>
+      <c r="B27" t="s">
+        <v>106</v>
+      </c>
+      <c r="D27" t="s">
+        <v>109</v>
+      </c>
+      <c r="E27" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="28" spans="1:5">
-      <c r="A28" s="3"/>
+      <c r="A28" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B28" t="s">
+        <v>111</v>
+      </c>
+      <c r="D28" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="29" spans="1:5">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B29" t="s">
+        <v>111</v>
+      </c>
+      <c r="D29" t="s">
+        <v>114</v>
+      </c>
+      <c r="E29" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="30" spans="1:5">
-      <c r="A30" s="3"/>
+      <c r="A30" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B30" t="s">
+        <v>111</v>
+      </c>
+      <c r="D30" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="31" spans="1:5">
-      <c r="A31" s="3"/>
+      <c r="A31" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B31" t="s">
+        <v>111</v>
+      </c>
+      <c r="D31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="32" spans="1:5">
-      <c r="A32" s="3"/>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" s="3"/>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" s="3"/>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" s="3"/>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" s="3"/>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" s="3"/>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="3"/>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" s="3"/>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="3"/>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" s="3"/>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" s="3"/>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" s="3"/>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" s="3"/>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" s="3"/>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" s="3"/>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" s="3"/>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" s="3"/>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" s="3"/>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" s="3"/>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" s="3"/>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" s="3"/>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" s="3"/>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" s="3"/>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" s="3"/>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" s="3"/>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" s="3"/>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" s="3"/>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" s="3"/>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" s="3"/>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" s="3"/>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" s="3"/>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" s="3"/>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" s="3"/>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" s="3"/>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" s="3"/>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" s="3"/>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" s="3"/>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" s="3"/>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" s="3"/>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" s="3"/>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" s="3"/>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" s="3"/>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" s="3"/>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" s="3"/>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" s="3"/>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" s="3"/>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" s="3"/>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" s="3"/>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" s="3"/>
-    </row>
-    <row r="102" spans="1:1">
+      <c r="A32" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B32" t="s">
+        <v>120</v>
+      </c>
+      <c r="D32" t="s">
+        <v>121</v>
+      </c>
+      <c r="E32" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B33" t="s">
+        <v>123</v>
+      </c>
+      <c r="D33" t="s">
+        <v>124</v>
+      </c>
+      <c r="E33" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D34" t="s">
+        <v>127</v>
+      </c>
+      <c r="E34" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D35" t="s">
+        <v>130</v>
+      </c>
+      <c r="E35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B36" t="s">
+        <v>132</v>
+      </c>
+      <c r="D36" t="s">
+        <v>133</v>
+      </c>
+      <c r="E36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B37" t="s">
+        <v>135</v>
+      </c>
+      <c r="D37" t="s">
+        <v>136</v>
+      </c>
+      <c r="E37" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>138</v>
+      </c>
+      <c r="E38" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B39" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" t="s">
+        <v>140</v>
+      </c>
+      <c r="E39" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B40" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" t="s">
+        <v>142</v>
+      </c>
+      <c r="E40" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B41" t="s">
+        <v>144</v>
+      </c>
+      <c r="D41" t="s">
+        <v>145</v>
+      </c>
+      <c r="E41" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B42" t="s">
+        <v>144</v>
+      </c>
+      <c r="D42" t="s">
+        <v>147</v>
+      </c>
+      <c r="E42" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B43" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" t="s">
+        <v>149</v>
+      </c>
+      <c r="E43" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" t="s">
+        <v>152</v>
+      </c>
+      <c r="E44" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E45" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B46" t="s">
+        <v>157</v>
+      </c>
+      <c r="D46" t="s">
+        <v>158</v>
+      </c>
+      <c r="E46" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B47" t="s">
+        <v>159</v>
+      </c>
+      <c r="D47" t="s">
+        <v>160</v>
+      </c>
+      <c r="E47" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B48" t="s">
+        <v>111</v>
+      </c>
+      <c r="D48" t="s">
+        <v>161</v>
+      </c>
+      <c r="E48" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B49" t="s">
+        <v>111</v>
+      </c>
+      <c r="D49" t="s">
+        <v>163</v>
+      </c>
+      <c r="E49" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B50" t="s">
+        <v>111</v>
+      </c>
+      <c r="D50" t="s">
+        <v>165</v>
+      </c>
+      <c r="E50" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B51" t="s">
+        <v>167</v>
+      </c>
+      <c r="D51" t="s">
+        <v>168</v>
+      </c>
+      <c r="E51" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B52" t="s">
+        <v>154</v>
+      </c>
+      <c r="D52" t="s">
+        <v>170</v>
+      </c>
+      <c r="E52" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B53" t="s">
+        <v>167</v>
+      </c>
+      <c r="D53" t="s">
+        <v>172</v>
+      </c>
+      <c r="E53" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B54" t="s">
+        <v>154</v>
+      </c>
+      <c r="D54" t="s">
+        <v>174</v>
+      </c>
+      <c r="E54" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B55" t="s">
+        <v>176</v>
+      </c>
+      <c r="D55" t="s">
+        <v>177</v>
+      </c>
+      <c r="E55" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B56" t="s">
+        <v>179</v>
+      </c>
+      <c r="D56" t="s">
+        <v>180</v>
+      </c>
+      <c r="E56" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B57" t="s">
+        <v>111</v>
+      </c>
+      <c r="D57" t="s">
+        <v>182</v>
+      </c>
+      <c r="E57" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B58" t="s">
+        <v>184</v>
+      </c>
+      <c r="D58" t="s">
+        <v>185</v>
+      </c>
+      <c r="E58" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B59" t="s">
+        <v>184</v>
+      </c>
+      <c r="D59" t="s">
+        <v>187</v>
+      </c>
+      <c r="E59" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B60" t="s">
+        <v>189</v>
+      </c>
+      <c r="D60" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B61" t="s">
+        <v>192</v>
+      </c>
+      <c r="D61" t="s">
+        <v>193</v>
+      </c>
+      <c r="E61" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B62" t="s">
+        <v>154</v>
+      </c>
+      <c r="D62" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B63" t="s">
+        <v>196</v>
+      </c>
+      <c r="D63" t="s">
+        <v>197</v>
+      </c>
+      <c r="E63" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B64" t="s">
+        <v>199</v>
+      </c>
+      <c r="D64" t="s">
+        <v>200</v>
+      </c>
+      <c r="E64" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B65" t="s">
+        <v>199</v>
+      </c>
+      <c r="D65" t="s">
+        <v>202</v>
+      </c>
+      <c r="E65" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D66" t="s">
+        <v>205</v>
+      </c>
+      <c r="E66" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B67" t="s">
+        <v>207</v>
+      </c>
+      <c r="D67" t="s">
+        <v>208</v>
+      </c>
+      <c r="E67" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B68" t="s">
+        <v>210</v>
+      </c>
+      <c r="D68" t="s">
+        <v>211</v>
+      </c>
+      <c r="E68" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B69" t="s">
+        <v>213</v>
+      </c>
+      <c r="D69" t="s">
+        <v>214</v>
+      </c>
+      <c r="E69" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B70" t="s">
+        <v>216</v>
+      </c>
+      <c r="D70" t="s">
+        <v>217</v>
+      </c>
+      <c r="E70" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B71" t="s">
+        <v>135</v>
+      </c>
+      <c r="D71" t="s">
+        <v>219</v>
+      </c>
+      <c r="E71" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B72" t="s">
+        <v>132</v>
+      </c>
+      <c r="D72" t="s">
+        <v>221</v>
+      </c>
+      <c r="E72" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B73" t="s">
+        <v>135</v>
+      </c>
+      <c r="D73" t="s">
+        <v>223</v>
+      </c>
+      <c r="E73" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B74" t="s">
+        <v>225</v>
+      </c>
+      <c r="D74" t="s">
+        <v>226</v>
+      </c>
+      <c r="E74" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B75" t="s">
+        <v>228</v>
+      </c>
+      <c r="D75" t="s">
+        <v>229</v>
+      </c>
+      <c r="E75" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B76" t="s">
+        <v>228</v>
+      </c>
+      <c r="D76" t="s">
+        <v>231</v>
+      </c>
+      <c r="E76" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B77" t="s">
+        <v>228</v>
+      </c>
+      <c r="D77" t="s">
+        <v>233</v>
+      </c>
+      <c r="E77" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B78" t="s">
+        <v>235</v>
+      </c>
+      <c r="D78" t="s">
+        <v>236</v>
+      </c>
+      <c r="E78" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B79" t="s">
+        <v>238</v>
+      </c>
+      <c r="D79" t="s">
+        <v>239</v>
+      </c>
+      <c r="E79" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B80" t="s">
+        <v>241</v>
+      </c>
+      <c r="D80" t="s">
+        <v>242</v>
+      </c>
+      <c r="E80" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B81" t="s">
+        <v>241</v>
+      </c>
+      <c r="D81" t="s">
+        <v>244</v>
+      </c>
+      <c r="E81" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B82" t="s">
+        <v>241</v>
+      </c>
+      <c r="D82" t="s">
+        <v>246</v>
+      </c>
+      <c r="E82" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B83" t="s">
+        <v>241</v>
+      </c>
+      <c r="D83" t="s">
+        <v>248</v>
+      </c>
+      <c r="E83" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B84" t="s">
+        <v>250</v>
+      </c>
+      <c r="D84" t="s">
+        <v>251</v>
+      </c>
+      <c r="E84" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B85" t="s">
+        <v>253</v>
+      </c>
+      <c r="D85" t="s">
+        <v>254</v>
+      </c>
+      <c r="E85" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B86" t="s">
+        <v>253</v>
+      </c>
+      <c r="D86" t="s">
+        <v>256</v>
+      </c>
+      <c r="E86" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B87" t="s">
+        <v>258</v>
+      </c>
+      <c r="D87" t="s">
+        <v>259</v>
+      </c>
+      <c r="E87" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B88" t="s">
+        <v>261</v>
+      </c>
+      <c r="D88" t="s">
+        <v>262</v>
+      </c>
+      <c r="E88" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B89" t="s">
+        <v>264</v>
+      </c>
+      <c r="D89" t="s">
+        <v>265</v>
+      </c>
+      <c r="E89" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B90" t="s">
+        <v>267</v>
+      </c>
+      <c r="D90" t="s">
+        <v>268</v>
+      </c>
+      <c r="E90" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B91" t="s">
+        <v>154</v>
+      </c>
+      <c r="D91" t="s">
+        <v>270</v>
+      </c>
+      <c r="E91" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B92" t="s">
+        <v>199</v>
+      </c>
+      <c r="D92" t="s">
+        <v>272</v>
+      </c>
+      <c r="E92" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B93" t="s">
+        <v>274</v>
+      </c>
+      <c r="D93" t="s">
+        <v>275</v>
+      </c>
+      <c r="E93" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B94" t="s">
+        <v>277</v>
+      </c>
+      <c r="D94" t="s">
+        <v>278</v>
+      </c>
+      <c r="E94" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B95" t="s">
+        <v>280</v>
+      </c>
+      <c r="D95" t="s">
+        <v>281</v>
+      </c>
+      <c r="E95" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B96" t="s">
+        <v>283</v>
+      </c>
+      <c r="D96" t="s">
+        <v>284</v>
+      </c>
+      <c r="E96" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B97" t="s">
+        <v>286</v>
+      </c>
+      <c r="D97" t="s">
+        <v>287</v>
+      </c>
+      <c r="E97" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B98" t="s">
+        <v>286</v>
+      </c>
+      <c r="D98" t="s">
+        <v>289</v>
+      </c>
+      <c r="E98" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B99" t="s">
+        <v>286</v>
+      </c>
+      <c r="D99" t="s">
+        <v>291</v>
+      </c>
+      <c r="E99" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B100" t="s">
+        <v>286</v>
+      </c>
+      <c r="D100" t="s">
+        <v>293</v>
+      </c>
+      <c r="E100" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" s="3">
+        <v>42303</v>
+      </c>
+      <c r="B101" t="s">
+        <v>295</v>
+      </c>
+      <c r="D101" t="s">
+        <v>296</v>
+      </c>
+      <c r="E101" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
       <c r="A102" s="3"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:5">
       <c r="A103" s="3"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:5">
       <c r="A104" s="3"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:5">
       <c r="A105" s="3"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:5">
       <c r="A106" s="3"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:5">
       <c r="A107" s="3"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:5">
       <c r="A108" s="3"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:5">
       <c r="A109" s="3"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:5">
       <c r="A110" s="3"/>
     </row>
-    <row r="111" spans="1:1">
+    <row r="111" spans="1:5">
       <c r="A111" s="3"/>
     </row>
-    <row r="112" spans="1:1">
+    <row r="112" spans="1:5">
       <c r="A112" s="3"/>
     </row>
     <row r="113" spans="1:1">

</xml_diff>